<commit_message>
edit Test case: customer pages #310
</commit_message>
<xml_diff>
--- a/Document/Reports/Report 5/Test case - PhucNH Customer app.xlsx
+++ b/Document/Reports/Report 5/Test case - PhucNH Customer app.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -55,9 +55,6 @@
     <t>CC3</t>
   </si>
   <si>
-    <t xml:space="preserve">Sytem show message error </t>
-  </si>
-  <si>
     <t>1.1. &lt;Customer&gt; Create New Contract</t>
   </si>
   <si>
@@ -85,15 +82,6 @@
     <t>Create new contract fail</t>
   </si>
   <si>
-    <t>Create contract with full information and pay online</t>
-  </si>
-  <si>
-    <t>Create contract with fail information</t>
-  </si>
-  <si>
-    <t>Create contract with full information but not pay online</t>
-  </si>
-  <si>
     <t>Renew contract success</t>
   </si>
   <si>
@@ -106,29 +94,7 @@
     <t>RC2</t>
   </si>
   <si>
-    <t>1. Prepare a contract with startdate: 7/25/2014 and expireddate: 7/25/2015 and status is "Ready"</t>
-  </si>
-  <si>
-    <t>System show page with message "renew success" and expired is updated "7/26/2016"</t>
-  </si>
-  <si>
-    <t>1. Prepare a contract with startdate: 7/11/2014 and expireddate: 7/11/2015 and status is "Expired"</t>
-  </si>
-  <si>
-    <t>System show page with message "renew success" and expired is updated "7/13/2016"</t>
-  </si>
-  <si>
-    <t>Renew contract</t>
-  </si>
-  <si>
-    <t>Create Contract
-- Print Card</t>
-  </si>
-  <si>
     <t>RC3</t>
-  </si>
-  <si>
-    <t>System show message error "Không được gia hạn trước 2 tháng"</t>
   </si>
   <si>
     <t>SCR1</t>
@@ -146,31 +112,10 @@
     <t>Send compensation fail</t>
   </si>
   <si>
-    <t>Input fail value into fied</t>
-  </si>
-  <si>
-    <t>System show error message depend on fail value input</t>
-  </si>
-  <si>
-    <t>Send compensation</t>
-  </si>
-  <si>
-    <t>Cancel contract</t>
-  </si>
-  <si>
     <t>Cancel contract success</t>
   </si>
   <si>
-    <t xml:space="preserve">Input right value into field </t>
-  </si>
-  <si>
     <t>Customer can see their new contract with status "No card" and some information about compensation, punishment, accident and card</t>
-  </si>
-  <si>
-    <t>Customer can see their new contract with status "Pending" and some information about compensation, punishment, accident and card</t>
-  </si>
-  <si>
-    <t>System will reload page and change status into "Request cancel" and show detail of request cancel</t>
   </si>
   <si>
     <t>Cancel contract fail</t>
@@ -179,44 +124,183 @@
     <t>Cancel contract contract fail</t>
   </si>
   <si>
-    <t>System will show error message "You must choose reason cancel before confirm"</t>
-  </si>
-  <si>
-    <t>1. Don't check any reason then click confirm</t>
-  </si>
-  <si>
-    <t>1. Prepare a contract with startdate:10/25/2014 and expireddate: 10/25/2015 and status is "Ready" and try to show button "Renew"</t>
-  </si>
-  <si>
     <t>CC4</t>
   </si>
   <si>
-    <t>RC4</t>
+    <t>Create new contract</t>
   </si>
   <si>
-    <t>1. Prepare a contrac with status Expired and login with another browser role "Staff" and do action renew contract in app customer and app staff</t>
+    <t>1. Create new contract with contract code "HD0001"
+2. Prepare a contract with startdate: 7/25/2014 and expireddate: 7/25/2015 and status is "Ready"
+3. Click "Gia hạn" button 
+4. Click "Gia hạn hợp đồng"
+5. Choose "Paypal" and login paypal to pay fee
+6. Click "Trở về trang chi tiết hợp đồng"</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Prepare a contract with status "Ready" check resson cancel </t>
+    <t xml:space="preserve">1. Create new contract with contract code "HD0001"
+2. Prepare a contract with startdate: 7/11/2014 and expireddate: 7/11/2015 and status is "Expired"
+3. Click "Gia hạn" button 
+4. Click "Gia hạn hợp đồng"
+5. Choose "Paypal" and login paypal to pay fee
+6. Click "Trở về trang chi tiết hợp đồng"
+</t>
   </si>
   <si>
-    <t>1. Prepare a contract with status "Ready" and login with another browser role "Staff" and do action cancel contract in app customer and app staff</t>
+    <t>System show page with message "Gia hạn thành công" and expired is updated "7/26/2016"</t>
   </si>
   <si>
-    <t>System will show error message "This action have been done by another person please try again"</t>
+    <t>System show page with message "Gia hạn thành công" and expired is updated "7/13/2016" and status change to "Ready"</t>
   </si>
   <si>
-    <t>1. Prepare a contract with status "Cancelled" and try to show button "Cancel"</t>
+    <t>1. Login with role customer
+1. Create new contract with contract code "HD0001" with 
+2. Prepare a contract with status Expired
+3. Open new browser and login with role Staff and goes into contract-detail at contract code "HD0001"
+4. Click "Gia hạn hợp đồng" at browser staff
+5. Do action like RC2
+6 Click "Gia hạn hợp đồng" at browser customer</t>
   </si>
   <si>
-    <t>System will show error message "You can not cancel the contract have been cancelled"</t>
+    <t xml:space="preserve">1. Create new contract with contract code "HD0001"
+2. Prepare a contract with status "Ready" check resson cancel
+3. Click "Hủy hợp đồng" button 
+4. Click " Xe cơ giới bị mất được cơ quan công an xác nhận"
+5. Click "Xác nhận" button  </t>
+  </si>
+  <si>
+    <t>System will reload page and change status into "Request cancel" and show detail of request cancel, show "Hủy yêu cầu button"</t>
+  </si>
+  <si>
+    <t>1. Login with role customer
+1. Create new contract with contract code "HD0001" with 
+2. Prepare a contract with status Ready
+3. Open new browser and login with role Staff and goes into contract-detail at contract code "HD0001"
+4. Click "Hủy hợp đồng" at browser staff
+5. Do action like CC1
+6. Click "Hủy hợp đồng" at browser customer</t>
+  </si>
+  <si>
+    <t>System will show error message "Thông tin hợp đồng đã bị sửa đổi trước đó bởi một người khác, vui lòng thực hiện lại thao tác"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Create new contract with contract code "HD0001"
+2. Prepare a contract with status "Ready" 
+3. Click "Hủy hợp đồng" button 
+4. Click "Xác nhận" button  </t>
+  </si>
+  <si>
+    <t>System will show error message "Vui lòng chọn lí do hủy hợp đồng trước khi xác nhận. Cảm ơn!"</t>
+  </si>
+  <si>
+    <t>1. Click "Hợp đồng mới" button.
+2. Input all default value according to Default form value.xlsx file" (Create new contract form)
+3. Click "Thêm hợp đồng"
+4. Click "Xác nhận"
+5. Click "Thanh toán ngay bây giờ"
+6. Login to paypla an pay fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click "Hợp đồng mới" button.
+2. Click "Thêm hợp đồng"
+</t>
+  </si>
+  <si>
+    <t>Sytem show message error and required input value</t>
+  </si>
+  <si>
+    <t>Default form value.xlsx file</t>
+  </si>
+  <si>
+    <t>1. Click "Hợp đồng mới" button.
+2. Input all default value according to Default form value.xlsx file" (Create new contract form)
+3. Click "Thêm hợp đồng"
+4. Click "Xác nhận"
+5. Click "Thanh toán ngay bây giờ"
+6. Click "Trực tiếp"</t>
+  </si>
+  <si>
+    <t>System shows map with detail address of company where customer can pay direct for their contract.
+Customer can see their new contract with status "Pending" and some information about compensation, punishment, accident and card</t>
+  </si>
+  <si>
+    <t>1. Create contract with contract code "HD0001"
+2. Click on "Hợp đồng" menu
+3. Search Contract with code "HD0001"
+4 Click link "HD0001"
+5. Click tab "Lịch sữ bồi thường"
+6. Click "Yêu cầu bồi thương"
+7. Input all default value according to Default form value.xlsx file" (Create new compensation) 
+8. Click "Gởi yêu cầu"
+9. Click "Trở về trang chi tiết hợp đồng"</t>
+  </si>
+  <si>
+    <t>Create new  contract
+Default form value.xlsx file</t>
+  </si>
+  <si>
+    <t>1. Create contract with contract code "HD0001"
+2. Click on "Hợp đồng" menu
+3. Search Contract with code "HD0001"
+4 Click link "HD0001"
+5. Click tab "Lịch sữ bồi thường"
+6. Click "Yêu cầu bồi thương"
+7. Input all default value according to Default form value.xlsx file" (Create new compensation) 
+8. Ngày xảy ra tai nạn input "09/13/2015"
+8. Click "Gởi yêu cầu"</t>
+  </si>
+  <si>
+    <t>System show error message "Ngày xảy ra tai nạn phải trước ngày hiện tại"</t>
+  </si>
+  <si>
+    <t>CNC4</t>
+  </si>
+  <si>
+    <t>1. Click "Hợp đồng mới" button.
+2. Input all default value according to Default form value.xlsx file" (Create new contract form)
+3. Thời điểm có hiệu lực input "07/04/2015"
+3. Click "Thêm hợp đồng"</t>
+  </si>
+  <si>
+    <t>Sytem show message error "Thời điểm có hiệu lực phải sau ngày hiện tại"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Create new contract with contract code "HD0001"
+2. Prepare a contract with status "Ready" 
+3. Click "Lý do khác" radio check 
+4. Click "Xác nhận" button  </t>
+  </si>
+  <si>
+    <t>CC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Create new contract with contract code "HD0001"
+2. Prepare a contract with status "Ready" 
+3. Click "Lý do khác" radio check 
+4. Input blank value into texterea 
+4. Click "Xác nhận" button  </t>
+  </si>
+  <si>
+    <t>SCR3</t>
+  </si>
+  <si>
+    <t>1. Create contract with contract code "HD0001"
+2. Click on "Hợp đồng" menu
+3. Search Contract with code "HD0001"
+4 Click link "HD0001"
+5. Click tab "Lịch sữ bồi thường"
+6. Click "Yêu cầu bồi thương"
+8. Click "Gởi yêu cầu"</t>
+  </si>
+  <si>
+    <t>System show error message "Vui lòng nhập giá trị" and required input into some field have "*" symbol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -226,10 +310,14 @@
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
@@ -241,6 +329,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="4">
@@ -275,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -304,7 +405,30 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,22 +739,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="113.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="115.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.28515625" customWidth="1"/>
+    <col min="4" max="4" width="66.140625" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -702,63 +826,63 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:26" s="16" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="15">
+        <v>42198</v>
+      </c>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+    </row>
+    <row r="4" spans="1:26" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>22</v>
+      <c r="C4" s="9" t="s">
+        <v>49</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="6">
-        <v>42198</v>
-      </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>12</v>
+      <c r="D4" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>8</v>
@@ -786,21 +910,21 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>20</v>
+      <c r="C5" s="9" t="s">
+        <v>52</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>49</v>
+      <c r="D5" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>8</v>
@@ -828,14 +952,28 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="6"/>
+    <row r="6" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="6">
+        <v>42198</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -856,9 +994,9 @@
       <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
+    <row r="7" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>13</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -886,7 +1024,7 @@
       <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
@@ -930,21 +1068,21 @@
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>8</v>
@@ -972,21 +1110,21 @@
       <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>8</v>
@@ -1014,21 +1152,21 @@
       <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>58</v>
+      <c r="C11" s="10" t="s">
+        <v>41</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>61</v>
+      <c r="D11" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>8</v>
@@ -1057,27 +1195,15 @@
       <c r="Z11" s="7"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>57</v>
+      <c r="A12" s="8" t="s">
+        <v>14</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="6">
-        <v>42198</v>
-      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -1099,16 +1225,30 @@
       <c r="Z12" s="7"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
+      <c r="A13" s="3" t="s">
+        <v>0</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -1128,31 +1268,29 @@
       <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>0</v>
+    <row r="14" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>9</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>1</v>
+      <c r="B14" s="5" t="s">
+        <v>31</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>2</v>
+      <c r="C14" s="10" t="s">
+        <v>42</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>3</v>
+      <c r="D14" s="10" t="s">
+        <v>43</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>4</v>
+      <c r="E14" s="9" t="s">
+        <v>36</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>5</v>
+      <c r="F14" s="5" t="s">
+        <v>8</v>
       </c>
-      <c r="G14" s="3" t="s">
-        <v>6</v>
+      <c r="G14" s="6">
+        <v>42198</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -1172,21 +1310,21 @@
       <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>59</v>
+      <c r="C15" s="10" t="s">
+        <v>44</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>50</v>
+      <c r="D15" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>8</v>
@@ -1214,21 +1352,21 @@
       <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>60</v>
+      <c r="C16" s="10" t="s">
+        <v>46</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>61</v>
+      <c r="D16" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>8</v>
@@ -1256,23 +1394,23 @@
       <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>52</v>
+      <c r="B17" s="7" t="s">
+        <v>34</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>54</v>
+      <c r="C17" s="10" t="s">
+        <v>61</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>53</v>
+      <c r="D17" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="7" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="6">
@@ -1298,22 +1436,28 @@
       <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
     </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>56</v>
+    <row r="18" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>62</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="D18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="6">
+        <v>42198</v>
+      </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -1336,7 +1480,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1408,21 +1552,21 @@
       <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>8</v>
@@ -1450,21 +1594,21 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>8</v>
@@ -1492,14 +1636,28 @@
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+    <row r="23" spans="1:26" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="6">
+        <v>42198</v>
+      </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>

</xml_diff>